<commit_message>
added method to get all videos from all channles from databse
75% done
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hardik\OneDrive\Documents\GitHub\YoutubeShortsToInstaReels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A743F6-8197-46EE-B4D9-4F294E72B91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A155B1A7-7176-4316-8CB6-D9C9CAB3153C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -410,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,41 +521,6 @@
       </c>
       <c r="C9" s="1" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
now script can print links to all videos of a channle
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hardik\OneDrive\Documents\GitHub\YoutubeShortsToInstaReels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A155B1A7-7176-4316-8CB6-D9C9CAB3153C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B46A6A-29B6-4D77-8DDC-E24EC30E2937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,12 +39,6 @@
     <t>sidemen shorts</t>
   </si>
   <si>
-    <t>https://www.youtube.com/c/SidemenShorts/videos</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/c/anthonypadilla2</t>
-  </si>
-  <si>
     <t>anthony padilla</t>
   </si>
   <si>
@@ -57,9 +51,6 @@
     <t>nile red</t>
   </si>
   <si>
-    <t>https://www.youtube.com/c/NileRedShorts</t>
-  </si>
-  <si>
     <t>ksi clips</t>
   </si>
   <si>
@@ -69,19 +60,28 @@
     <t>impalsive clips</t>
   </si>
   <si>
-    <t>https://www.youtube.com/c/ImpaulsiveClips</t>
-  </si>
-  <si>
     <t>w2s clips</t>
   </si>
   <si>
-    <t>https://www.youtube.com/c/W2SClips</t>
-  </si>
-  <si>
     <t>smosh shorts</t>
   </si>
   <si>
-    <t>https://www.youtube.com/c/smoshshorts</t>
+    <t>https://www.youtube.com/c/UCbAZH3nTxzyNmehmTUhuUsA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/c/UCPJHQ5_DLtxZ1gzBvZE99_g</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/c/UCA0mlN90EHCizvo101nbr-g</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/c/UCE9ZKI1b_PhVm3gejYuilhw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/c/UCZiJzk4wTIzaqHI4FXZ_eRQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/c/UCS_NmOvbqaC9ccWSymx5Gpg</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +443,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -451,10 +451,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -462,10 +462,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -473,10 +473,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -484,10 +484,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -495,10 +495,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -506,10 +506,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -517,7 +517,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
made database of all videos from given channles
now i have to filter these results and make the database more informative
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hardik\OneDrive\Documents\GitHub\YoutubeShortsToInstaReels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B46A6A-29B6-4D77-8DDC-E24EC30E2937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF391CA0-2C89-49AA-AE50-3792DCE60715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>link to channle</t>
   </si>
@@ -39,12 +39,6 @@
     <t>sidemen shorts</t>
   </si>
   <si>
-    <t>anthony padilla</t>
-  </si>
-  <si>
-    <t>mr beast</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/channel/UC4-79UOlP48-QNGgCko5p2g</t>
   </si>
   <si>
@@ -69,9 +63,6 @@
     <t>https://www.youtube.com/c/UCbAZH3nTxzyNmehmTUhuUsA</t>
   </si>
   <si>
-    <t>https://www.youtube.com/c/UCPJHQ5_DLtxZ1gzBvZE99_g</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/c/UCA0mlN90EHCizvo101nbr-g</t>
   </si>
   <si>
@@ -82,6 +73,33 @@
   </si>
   <si>
     <t>https://www.youtube.com/c/UCS_NmOvbqaC9ccWSymx5Gpg</t>
+  </si>
+  <si>
+    <t>mr beast shorts</t>
+  </si>
+  <si>
+    <t>link to user instagram</t>
+  </si>
+  <si>
+    <t>sidemen</t>
+  </si>
+  <si>
+    <t>mrbeast</t>
+  </si>
+  <si>
+    <t>nile.red</t>
+  </si>
+  <si>
+    <t>ksi</t>
+  </si>
+  <si>
+    <t>impaulsiveshow</t>
+  </si>
+  <si>
+    <t>wroetoshaw</t>
+  </si>
+  <si>
+    <t>smosh</t>
   </si>
 </sst>
 </file>
@@ -410,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +442,7 @@
     <col min="4" max="4" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -434,8 +452,11 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -443,21 +464,27 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -465,21 +492,27 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -487,52 +520,49 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{DA719BF5-FF72-4663-B8A4-7199C46404C1}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{CA7C9B98-BA97-4B98-9E7D-847773C772BD}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{569973E8-9A15-40E4-854E-5564D8596F2C}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{59395733-6BBE-4CA8-A148-43B2AC0B0A15}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{DB8F9967-CBA2-4E15-B367-1307D632C6D9}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{FF9496DF-13E7-40DE-A111-4A06B6B49621}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{583BFC79-F445-40B5-BC02-A607ECD7EA2A}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{4BE92838-C7E1-4836-BB45-963046ED14C5}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{569973E8-9A15-40E4-854E-5564D8596F2C}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{59395733-6BBE-4CA8-A148-43B2AC0B0A15}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{DB8F9967-CBA2-4E15-B367-1307D632C6D9}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{FF9496DF-13E7-40DE-A111-4A06B6B49621}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{583BFC79-F445-40B5-BC02-A607ECD7EA2A}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{4BE92838-C7E1-4836-BB45-963046ED14C5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>